<commit_message>
minor fix export report
</commit_message>
<xml_diff>
--- a/HotelManagement/Assets/XLSXTemplate/Report_template.xlsx
+++ b/HotelManagement/Assets/XLSXTemplate/Report_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Deadlines\Year 3\Semester II_3\Software Design\Project\HotelManagement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\third year\Sem2\TKPM\HotelManagement\HotelManagement\Assets\XLSXTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D31824-F2FB-43E2-B1D6-A2C53AF154E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CED4137-2B2E-48CE-9DBA-2E2015627BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30465" yWindow="1785" windowWidth="25890" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revenue Report" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="_([$VND]\ * #,##0_);_([$VND]\ * \(#,##0\);_([$VND]\ * &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_([$VND]\ * #,##0_);_([$VND]\ * \(#,##0\);_([$VND]\ * &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -162,7 +162,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -170,46 +170,41 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -509,42 +504,42 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="4"/>
+      <c r="A1" s="4"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="14"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="4"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="14"/>
     </row>
     <row r="5" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -553,22 +548,22 @@
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D6" s="11"/>
+      <c r="D6" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="A6:D1048576">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -582,42 +577,42 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="4"/>
+      <c r="A1" s="4"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="14"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="4"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="14"/>
     </row>
     <row r="5" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -626,15 +621,15 @@
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D6" s="11"/>
+      <c r="D6" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>